<commit_message>
Corrected mistake on allocated lead
Corrected mistake on allocated lead
</commit_message>
<xml_diff>
--- a/Jubilee_Line_website 1.xlsx
+++ b/Jubilee_Line_website 1.xlsx
@@ -12,8 +12,10 @@
     <sheet name="Cocktail bars" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Cocktail bars'!$A$1:$D$29</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Cocktail bars'!$A$1:$D$26</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Cocktail bars'!$A$1:$D$26</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Final Choice'!$A$1:$F$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Cocktail bars'!$A$1:$D$29</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Cocktail bars'!$A$1:$D$26</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -541,20 +543,24 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.6009389671362"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5117370892019"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -570,14 +576,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>6</v>
       </c>
@@ -597,7 +603,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>12</v>
       </c>
@@ -637,7 +643,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>22</v>
       </c>
@@ -657,7 +663,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>26</v>
       </c>
@@ -677,7 +683,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>30</v>
       </c>
@@ -694,7 +700,7 @@
         <v>29</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -714,10 +720,10 @@
         <v>29</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>36</v>
       </c>
@@ -757,7 +763,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>43</v>
       </c>
@@ -778,6 +784,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F11">
+    <filterColumn colId="5">
+      <customFilters and="true">
+        <customFilter operator="equal" val="Cindy"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="https://www.google.co.uk/maps/dir/''/''/@51.5416164,-0.0712982,12z/data=!3m1!4b1!4m8!4m7!1m0!1m5!1m1!1s0x48761d62192c7035:0x20db3737246b79a5!2m2!1d-0.0012587!2d51.5416372"/>
     <hyperlink ref="C9" r:id="rId2" display="https://www.google.co.uk/maps/place/Wired+co./@51.5467912,-0.1908584,17.99z/data=!4m8!1m2!2m1!1sWired+coffee!3m4!1s0x48761079cce65a13:0xcbe303667f98bd54!8m2!3d51.5464816!4d-0.1905667"/>
@@ -792,6 +805,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -808,11 +822,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4460093896714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.9483568075117"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.4553990610329"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.6572769953052"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="13.5962441314554"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.9014084507042"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.150234741784"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.169014084507"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.0469483568075"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="14.8544600938967"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1238,7 +1252,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:D29">
+  <autoFilter ref="A1:D26">
     <filterColumn colId="1">
       <filters>
         <filter val="London Bridge"/>

</xml_diff>